<commit_message>
New Data - Issue Fixed
</commit_message>
<xml_diff>
--- a/data_raw/medgemma.xlsx
+++ b/data_raw/medgemma.xlsx
@@ -699,7 +699,7 @@
           <t>CHIEF COMPLAINT
   Left wrist and hand pain.
   HISTORY OF PRESENT ILLNESS
-  George Lewis is a pleasant 57-year-old male who presents to the clinic today for evaluation of left wrist and hand pain. He reports an onset of a few months ago but denies any specific injury. However, the patient notes he often engages in repetitive motions while performing his work duties. His symptoms are worse at night, and he wakes with numbness in the bilateral hands. He experiences numbness in all fingers, but states it is the most noticeable in the left thumb and index finger. He affirms intermittent numbness in the left little finger. For relief, he shakes his hands upon waking. The patient also experiences weakness in his left hand. He reports he drops objects and explains â€œI have a hard time feeling it.â€_x009d_
+  George Lewis is a pleasant 57-year-old male who presents to the clinic today for evaluation of left wrist and hand pain. He reports an onset of a few months ago but denies any specific injury. However, the patient notes he often engages in repetitive motions while performing his work duties. His symptoms are worse at night, and he wakes with numbness in the bilateral hands. He experiences numbness in all fingers, but states it is the most noticeable in the left thumb and index finger. He affirms intermittent numbness in the left little finger. For relief, he shakes his hands upon waking. The patient also experiences weakness in his left hand. He reports he drops objects and explains â€œI have a hard time feeling it.â€
   MEDICAL HISTORY
   The patient denies a history of rheumatoid arthritis.
   SOCIAL HISTORY
@@ -2205,7 +2205,11 @@
   The patient will follow up with me after his MRI for results.</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>test1_aci_asrcorr</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>[ڈاکٹر] ہی برانڈن، آپ کو آج یہاں دیکھ کر خوشی ہوئی۔ مجھے آپ کے ریکارڈ میں نظر آیا ہے کہ آپ کو گردن میں کچھ درد ہو رہا ہے۔ کیا آپ مجھے بتا سکتے ہیں کہ کیا ہوا؟
@@ -2400,7 +2404,11 @@
   The patient will follow up with me in 2 weeks to assess his progress and for possible repeat debridement. He has been advised to call the office if his symptoms worsen and we will get him in sooner, however, if he starts to develop a fever or necrosis he has been instructed to go to the ER.</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>test1_aci_asrcorr</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>[ڈاکٹر] ہی گریگوری، آج آپ سے مل کر خوشی ہوئی۔ تو میرے نوٹس دیکھیں۔ مجھے پتہ چلا ہے کہ آپ یہاں آئے ہیں کیونکہ آپ کو ٹھیک نہ ہونے والا پاؤں کا السر ہے۔ کیا آپ مجھے بتا سکتے ہیں کہ آپ کی حالت کیسی ہے؟ یہ کب سے ہے؟ اس کے ساتھ کیا مسئلہ ہے؟

</xml_diff>